<commit_message>
Update Les différents accents du français - November 1 2021 - ENG for Shuyi.xlsx
</commit_message>
<xml_diff>
--- a/Data/Les différents accents du français - November 1 2021 - ENG for Shuyi.xlsx
+++ b/Data/Les différents accents du français - November 1 2021 - ENG for Shuyi.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20380"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marie\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shuyitan/Desktop/Consulting/Linguistic_Consulting/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F236AD-663D-4EF3-B9B3-D32F570EBDCE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7AC2EA0-56A9-8E40-834C-3DDBFFC87F52}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19200" windowHeight="8160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet0" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6361" uniqueCount="1600">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6329" uniqueCount="1600">
   <si>
     <t>ResponseId</t>
   </si>
@@ -5216,21 +5216,21 @@
   <dimension ref="A1:EQ159"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="EP3" sqref="EP3"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="11" max="11" width="10.7265625" customWidth="1"/>
-    <col min="12" max="12" width="13.6328125" customWidth="1"/>
-    <col min="13" max="13" width="11.36328125" customWidth="1"/>
-    <col min="14" max="14" width="14.54296875" customWidth="1"/>
-    <col min="146" max="146" width="24.7265625" customWidth="1"/>
-    <col min="147" max="147" width="46.36328125" customWidth="1"/>
+    <col min="11" max="11" width="10.6640625" customWidth="1"/>
+    <col min="12" max="12" width="13.6640625" customWidth="1"/>
+    <col min="13" max="13" width="11.33203125" customWidth="1"/>
+    <col min="14" max="14" width="14.5" customWidth="1"/>
+    <col min="146" max="146" width="24.6640625" customWidth="1"/>
+    <col min="147" max="147" width="46.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:147" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:147" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -5669,7 +5669,7 @@
       </c>
       <c r="EQ1" s="2"/>
     </row>
-    <row r="2" spans="1:147" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:147" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>143</v>
       </c>
@@ -6106,7 +6106,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="3" spans="1:147" ht="261" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:147" ht="288" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>277</v>
       </c>
@@ -6547,7 +6547,7 @@
         <v>1599</v>
       </c>
     </row>
-    <row r="4" spans="1:147" ht="87" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:147" ht="96" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>295</v>
       </c>
@@ -6987,7 +6987,7 @@
         <v>1573</v>
       </c>
     </row>
-    <row r="5" spans="1:147" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:147" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>312</v>
       </c>
@@ -7427,7 +7427,7 @@
         <v>1573</v>
       </c>
     </row>
-    <row r="6" spans="1:147" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:147" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>322</v>
       </c>
@@ -7867,7 +7867,7 @@
         <v>1577</v>
       </c>
     </row>
-    <row r="7" spans="1:147" ht="87" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:147" ht="96" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>335</v>
       </c>
@@ -8307,7 +8307,7 @@
         <v>1573</v>
       </c>
     </row>
-    <row r="8" spans="1:147" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:147" ht="112" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>350</v>
       </c>
@@ -8747,7 +8747,7 @@
         <v>1573</v>
       </c>
     </row>
-    <row r="9" spans="1:147" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:147" ht="160" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>359</v>
       </c>
@@ -9187,7 +9187,7 @@
         <v>1576</v>
       </c>
     </row>
-    <row r="10" spans="1:147" ht="203" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:147" ht="224" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>375</v>
       </c>
@@ -9627,7 +9627,7 @@
         <v>1591</v>
       </c>
     </row>
-    <row r="11" spans="1:147" ht="116" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:147" ht="112" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>386</v>
       </c>
@@ -10064,7 +10064,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="12" spans="1:147" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:147" ht="144" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>400</v>
       </c>
@@ -10504,7 +10504,7 @@
         <v>1592</v>
       </c>
     </row>
-    <row r="13" spans="1:147" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:147" ht="160" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>413</v>
       </c>
@@ -10944,7 +10944,7 @@
         <v>1574</v>
       </c>
     </row>
-    <row r="14" spans="1:147" ht="145" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:147" ht="144" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>422</v>
       </c>
@@ -11381,7 +11381,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="15" spans="1:147" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:147" ht="208" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>436</v>
       </c>
@@ -11819,7 +11819,7 @@
         <v>1593</v>
       </c>
     </row>
-    <row r="16" spans="1:147" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:147" ht="160" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>446</v>
       </c>
@@ -12256,7 +12256,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="17" spans="1:146" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:146" ht="48" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>454</v>
       </c>
@@ -12696,7 +12696,7 @@
         <v>1576</v>
       </c>
     </row>
-    <row r="18" spans="1:146" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:146" ht="112" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>459</v>
       </c>
@@ -13136,7 +13136,7 @@
         <v>1577</v>
       </c>
     </row>
-    <row r="19" spans="1:146" ht="58" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:146" ht="64" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>470</v>
       </c>
@@ -13573,7 +13573,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="20" spans="1:146" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:146" ht="160" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>476</v>
       </c>
@@ -14010,7 +14010,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="21" spans="1:146" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:146" ht="48" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>485</v>
       </c>
@@ -14447,7 +14447,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="22" spans="1:146" ht="58" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:146" ht="64" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>490</v>
       </c>
@@ -14887,7 +14887,7 @@
         <v>1573</v>
       </c>
     </row>
-    <row r="23" spans="1:146" ht="58" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:146" ht="64" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>497</v>
       </c>
@@ -15322,7 +15322,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="24" spans="1:146" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:146" ht="112" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>505</v>
       </c>
@@ -15762,7 +15762,7 @@
         <v>1573</v>
       </c>
     </row>
-    <row r="25" spans="1:146" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:146" ht="48" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>516</v>
       </c>
@@ -16199,7 +16199,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="26" spans="1:146" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:146" ht="48" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>521</v>
       </c>
@@ -16636,7 +16636,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="27" spans="1:146" ht="116" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:146" ht="112" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>524</v>
       </c>
@@ -17076,7 +17076,7 @@
         <v>1573</v>
       </c>
     </row>
-    <row r="28" spans="1:146" ht="58" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:146" ht="48" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>534</v>
       </c>
@@ -17513,7 +17513,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="29" spans="1:146" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:146" ht="112" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>544</v>
       </c>
@@ -17953,7 +17953,7 @@
         <v>1573</v>
       </c>
     </row>
-    <row r="30" spans="1:146" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:146" ht="144" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>557</v>
       </c>
@@ -18390,7 +18390,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="31" spans="1:146" ht="58" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:146" ht="64" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>565</v>
       </c>
@@ -18830,7 +18830,7 @@
         <v>1576</v>
       </c>
     </row>
-    <row r="32" spans="1:146" ht="87" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:146" ht="80" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>571</v>
       </c>
@@ -19267,7 +19267,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="33" spans="1:146" ht="116" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:146" ht="112" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>582</v>
       </c>
@@ -19707,7 +19707,7 @@
         <v>1573</v>
       </c>
     </row>
-    <row r="34" spans="1:146" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:146" ht="48" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>588</v>
       </c>
@@ -20147,7 +20147,7 @@
         <v>1573</v>
       </c>
     </row>
-    <row r="35" spans="1:146" ht="58" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:146" ht="48" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>594</v>
       </c>
@@ -20587,7 +20587,7 @@
         <v>1573</v>
       </c>
     </row>
-    <row r="36" spans="1:146" ht="145" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:146" ht="160" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>602</v>
       </c>
@@ -21027,7 +21027,7 @@
         <v>1576</v>
       </c>
     </row>
-    <row r="37" spans="1:146" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:146" ht="192" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>609</v>
       </c>
@@ -21467,7 +21467,7 @@
         <v>1594</v>
       </c>
     </row>
-    <row r="38" spans="1:146" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:146" ht="96" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>621</v>
       </c>
@@ -21904,7 +21904,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="39" spans="1:146" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:146" ht="80" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>637</v>
       </c>
@@ -22344,7 +22344,7 @@
         <v>1581</v>
       </c>
     </row>
-    <row r="40" spans="1:146" ht="87" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:146" ht="96" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>644</v>
       </c>
@@ -22784,7 +22784,7 @@
         <v>1582</v>
       </c>
     </row>
-    <row r="41" spans="1:146" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:146" ht="48" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>652</v>
       </c>
@@ -23224,7 +23224,7 @@
         <v>1585</v>
       </c>
     </row>
-    <row r="42" spans="1:146" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:146" ht="48" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>657</v>
       </c>
@@ -23664,7 +23664,7 @@
         <v>1573</v>
       </c>
     </row>
-    <row r="43" spans="1:146" ht="58" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:146" ht="64" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>662</v>
       </c>
@@ -24104,7 +24104,7 @@
         <v>1576</v>
       </c>
     </row>
-    <row r="44" spans="1:146" ht="87" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:146" ht="96" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>669</v>
       </c>
@@ -24541,7 +24541,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="45" spans="1:146" ht="58" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:146" ht="64" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>677</v>
       </c>
@@ -24981,7 +24981,7 @@
         <v>1573</v>
       </c>
     </row>
-    <row r="46" spans="1:146" ht="58" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:146" ht="48" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>682</v>
       </c>
@@ -25418,7 +25418,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="47" spans="1:146" ht="145" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:146" ht="128" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>687</v>
       </c>
@@ -25858,7 +25858,7 @@
         <v>1573</v>
       </c>
     </row>
-    <row r="48" spans="1:146" ht="87" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:146" ht="64" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>696</v>
       </c>
@@ -26298,7 +26298,7 @@
         <v>1573</v>
       </c>
     </row>
-    <row r="49" spans="1:146" ht="58" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:146" ht="64" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>703</v>
       </c>
@@ -26738,7 +26738,7 @@
         <v>1436</v>
       </c>
     </row>
-    <row r="50" spans="1:146" ht="87" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:146" ht="96" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>710</v>
       </c>
@@ -27178,7 +27178,7 @@
         <v>1586</v>
       </c>
     </row>
-    <row r="51" spans="1:146" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:146" ht="64" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>721</v>
       </c>
@@ -27618,7 +27618,7 @@
         <v>1576</v>
       </c>
     </row>
-    <row r="52" spans="1:146" ht="58" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:146" ht="64" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>728</v>
       </c>
@@ -28055,7 +28055,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="53" spans="1:146" ht="58" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:146" ht="48" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>738</v>
       </c>
@@ -28492,7 +28492,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="54" spans="1:146" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:146" ht="80" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>742</v>
       </c>
@@ -28929,7 +28929,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="55" spans="1:146" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:146" ht="80" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>749</v>
       </c>
@@ -29366,7 +29366,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="56" spans="1:146" ht="58" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:146" ht="48" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>759</v>
       </c>
@@ -29806,7 +29806,7 @@
         <v>1576</v>
       </c>
     </row>
-    <row r="57" spans="1:146" ht="58" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:146" ht="48" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>769</v>
       </c>
@@ -30243,7 +30243,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="58" spans="1:146" ht="58" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:146" ht="64" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>774</v>
       </c>
@@ -30683,7 +30683,7 @@
         <v>1573</v>
       </c>
     </row>
-    <row r="59" spans="1:146" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:146" ht="48" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>779</v>
       </c>
@@ -31123,7 +31123,7 @@
         <v>1573</v>
       </c>
     </row>
-    <row r="60" spans="1:146" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:146" ht="112" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>785</v>
       </c>
@@ -31560,7 +31560,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="61" spans="1:146" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:146" ht="128" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>792</v>
       </c>
@@ -32000,7 +32000,7 @@
         <v>1573</v>
       </c>
     </row>
-    <row r="62" spans="1:146" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:146" ht="80" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>802</v>
       </c>
@@ -32440,7 +32440,7 @@
         <v>1573</v>
       </c>
     </row>
-    <row r="63" spans="1:146" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:146" ht="144" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>809</v>
       </c>
@@ -32880,7 +32880,7 @@
         <v>1576</v>
       </c>
     </row>
-    <row r="64" spans="1:146" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:146" ht="48" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>817</v>
       </c>
@@ -33320,7 +33320,7 @@
         <v>1576</v>
       </c>
     </row>
-    <row r="65" spans="1:146" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:146" ht="144" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>822</v>
       </c>
@@ -33760,7 +33760,7 @@
         <v>1587</v>
       </c>
     </row>
-    <row r="66" spans="1:146" ht="203" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:146" ht="224" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>833</v>
       </c>
@@ -34198,7 +34198,7 @@
         <v>1576</v>
       </c>
     </row>
-    <row r="67" spans="1:146" ht="87" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:146" ht="96" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>844</v>
       </c>
@@ -34638,7 +34638,7 @@
         <v>1590</v>
       </c>
     </row>
-    <row r="68" spans="1:146" ht="58" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:146" ht="64" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>854</v>
       </c>
@@ -35078,7 +35078,7 @@
         <v>1573</v>
       </c>
     </row>
-    <row r="69" spans="1:146" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:146" ht="96" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>858</v>
       </c>
@@ -35515,7 +35515,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="70" spans="1:146" ht="348" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:146" ht="350" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>869</v>
       </c>
@@ -35955,7 +35955,7 @@
         <v>1573</v>
       </c>
     </row>
-    <row r="71" spans="1:146" ht="58" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:146" ht="64" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>882</v>
       </c>
@@ -36395,7 +36395,7 @@
         <v>1590</v>
       </c>
     </row>
-    <row r="72" spans="1:146" ht="58" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:146" ht="64" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>886</v>
       </c>
@@ -36832,7 +36832,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="73" spans="1:146" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:146" ht="48" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>891</v>
       </c>
@@ -37272,7 +37272,7 @@
         <v>1595</v>
       </c>
     </row>
-    <row r="74" spans="1:146" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:146" ht="48" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>898</v>
       </c>
@@ -37709,7 +37709,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="75" spans="1:146" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:146" ht="144" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>904</v>
       </c>
@@ -38149,7 +38149,7 @@
         <v>1584</v>
       </c>
     </row>
-    <row r="76" spans="1:146" ht="203" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:146" ht="192" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>913</v>
       </c>
@@ -38589,7 +38589,7 @@
         <v>1596</v>
       </c>
     </row>
-    <row r="77" spans="1:146" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:146" ht="112" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>925</v>
       </c>
@@ -39029,7 +39029,7 @@
         <v>1590</v>
       </c>
     </row>
-    <row r="78" spans="1:146" ht="145" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:146" ht="160" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>931</v>
       </c>
@@ -39469,7 +39469,7 @@
         <v>1573</v>
       </c>
     </row>
-    <row r="79" spans="1:146" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:146" ht="48" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>941</v>
       </c>
@@ -39906,7 +39906,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="80" spans="1:146" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:146" ht="48" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>946</v>
       </c>
@@ -40343,7 +40343,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="81" spans="1:146" ht="87" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:146" ht="96" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>953</v>
       </c>
@@ -40780,7 +40780,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="82" spans="1:146" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:146" ht="144" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>958</v>
       </c>
@@ -41217,7 +41217,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="83" spans="1:146" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:146" ht="48" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>968</v>
       </c>
@@ -41657,7 +41657,7 @@
         <v>1576</v>
       </c>
     </row>
-    <row r="84" spans="1:146" ht="58" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:146" ht="48" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>971</v>
       </c>
@@ -42097,7 +42097,7 @@
         <v>1590</v>
       </c>
     </row>
-    <row r="85" spans="1:146" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:146" ht="48" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>975</v>
       </c>
@@ -42534,7 +42534,7 @@
         <v>977</v>
       </c>
     </row>
-    <row r="86" spans="1:146" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:146" ht="80" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>978</v>
       </c>
@@ -42974,7 +42974,7 @@
         <v>1576</v>
       </c>
     </row>
-    <row r="87" spans="1:146" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:146" ht="144" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>985</v>
       </c>
@@ -43414,7 +43414,7 @@
         <v>1573</v>
       </c>
     </row>
-    <row r="88" spans="1:146" ht="58" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:146" ht="64" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>994</v>
       </c>
@@ -43854,7 +43854,7 @@
         <v>1573</v>
       </c>
     </row>
-    <row r="89" spans="1:146" ht="87" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:146" ht="96" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>1001</v>
       </c>
@@ -44294,7 +44294,7 @@
         <v>1584</v>
       </c>
     </row>
-    <row r="90" spans="1:146" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:146" ht="48" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>1012</v>
       </c>
@@ -44734,7 +44734,7 @@
         <v>1573</v>
       </c>
     </row>
-    <row r="91" spans="1:146" ht="275.5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:146" ht="256" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>1016</v>
       </c>
@@ -45171,7 +45171,7 @@
         <v>1031</v>
       </c>
     </row>
-    <row r="92" spans="1:146" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:146" ht="64" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>1032</v>
       </c>
@@ -45608,7 +45608,7 @@
         <v>1043</v>
       </c>
     </row>
-    <row r="93" spans="1:146" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:146" ht="80" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>1044</v>
       </c>
@@ -46045,7 +46045,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="94" spans="1:146" ht="58" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:146" ht="48" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>1050</v>
       </c>
@@ -46485,7 +46485,7 @@
         <v>1573</v>
       </c>
     </row>
-    <row r="95" spans="1:146" ht="87" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:146" ht="96" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>1054</v>
       </c>
@@ -46922,7 +46922,7 @@
         <v>1062</v>
       </c>
     </row>
-    <row r="96" spans="1:146" ht="58" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:146" ht="48" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>1063</v>
       </c>
@@ -47359,7 +47359,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="97" spans="1:146" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:146" ht="112" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>1067</v>
       </c>
@@ -47796,7 +47796,7 @@
         <v>1072</v>
       </c>
     </row>
-    <row r="98" spans="1:146" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:146" ht="48" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>1073</v>
       </c>
@@ -48236,7 +48236,7 @@
         <v>1576</v>
       </c>
     </row>
-    <row r="99" spans="1:146" ht="58" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:146" ht="64" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>1077</v>
       </c>
@@ -48673,7 +48673,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="100" spans="1:146" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:146" ht="80" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>1082</v>
       </c>
@@ -49110,7 +49110,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="101" spans="1:146" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:146" ht="112" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>1088</v>
       </c>
@@ -49550,7 +49550,7 @@
         <v>1576</v>
       </c>
     </row>
-    <row r="102" spans="1:146" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:146" ht="112" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>1098</v>
       </c>
@@ -49990,7 +49990,7 @@
         <v>1573</v>
       </c>
     </row>
-    <row r="103" spans="1:146" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:146" ht="112" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>1105</v>
       </c>
@@ -50427,7 +50427,7 @@
         <v>1110</v>
       </c>
     </row>
-    <row r="104" spans="1:146" ht="58" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:146" ht="64" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>1111</v>
       </c>
@@ -50867,7 +50867,7 @@
         <v>1578</v>
       </c>
     </row>
-    <row r="105" spans="1:146" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:146" ht="48" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>1126</v>
       </c>
@@ -51304,7 +51304,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="106" spans="1:146" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:146" ht="48" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>1130</v>
       </c>
@@ -51744,7 +51744,7 @@
         <v>1589</v>
       </c>
     </row>
-    <row r="107" spans="1:146" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:146" ht="112" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>1133</v>
       </c>
@@ -52184,7 +52184,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="108" spans="1:146" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:146" ht="160" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>1139</v>
       </c>
@@ -52621,7 +52621,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="109" spans="1:146" ht="58" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:146" ht="64" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>1142</v>
       </c>
@@ -53061,7 +53061,7 @@
         <v>1573</v>
       </c>
     </row>
-    <row r="110" spans="1:146" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:146" ht="112" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>1150</v>
       </c>
@@ -53498,7 +53498,7 @@
         <v>1155</v>
       </c>
     </row>
-    <row r="111" spans="1:146" ht="58" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:146" ht="64" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>1156</v>
       </c>
@@ -53935,7 +53935,7 @@
         <v>1160</v>
       </c>
     </row>
-    <row r="112" spans="1:146" ht="58" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:146" ht="64" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>1161</v>
       </c>
@@ -54375,7 +54375,7 @@
         <v>1576</v>
       </c>
     </row>
-    <row r="113" spans="1:146" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:146" ht="112" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>1169</v>
       </c>
@@ -54812,7 +54812,7 @@
         <v>1173</v>
       </c>
     </row>
-    <row r="114" spans="1:146" ht="87" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:146" ht="64" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>1174</v>
       </c>
@@ -55252,7 +55252,7 @@
         <v>1579</v>
       </c>
     </row>
-    <row r="115" spans="1:146" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:146" ht="96" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>1178</v>
       </c>
@@ -55692,7 +55692,7 @@
         <v>1576</v>
       </c>
     </row>
-    <row r="116" spans="1:146" ht="87" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:146" ht="96" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>1182</v>
       </c>
@@ -56132,7 +56132,7 @@
         <v>1589</v>
       </c>
     </row>
-    <row r="117" spans="1:146" ht="145" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:146" ht="144" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>1187</v>
       </c>
@@ -56572,7 +56572,7 @@
         <v>1573</v>
       </c>
     </row>
-    <row r="118" spans="1:146" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:146" ht="48" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>1197</v>
       </c>
@@ -57012,7 +57012,7 @@
         <v>1589</v>
       </c>
     </row>
-    <row r="119" spans="1:146" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:146" ht="80" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>1205</v>
       </c>
@@ -57449,7 +57449,7 @@
         <v>1214</v>
       </c>
     </row>
-    <row r="120" spans="1:146" ht="174" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:146" ht="176" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>1215</v>
       </c>
@@ -57887,7 +57887,7 @@
         <v>1573</v>
       </c>
     </row>
-    <row r="121" spans="1:146" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:146" ht="48" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>1230</v>
       </c>
@@ -58327,7 +58327,7 @@
         <v>1582</v>
       </c>
     </row>
-    <row r="122" spans="1:146" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:146" ht="80" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>1236</v>
       </c>
@@ -58764,7 +58764,7 @@
         <v>1240</v>
       </c>
     </row>
-    <row r="123" spans="1:146" ht="58" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:146" ht="64" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>1241</v>
       </c>
@@ -59201,7 +59201,7 @@
         <v>1243</v>
       </c>
     </row>
-    <row r="124" spans="1:146" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:146" ht="48" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>1244</v>
       </c>
@@ -59638,7 +59638,7 @@
         <v>1246</v>
       </c>
     </row>
-    <row r="125" spans="1:146" ht="145" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:146" ht="144" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>1247</v>
       </c>
@@ -60075,7 +60075,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="126" spans="1:146" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:146" ht="48" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>1259</v>
       </c>
@@ -60515,7 +60515,7 @@
         <v>1597</v>
       </c>
     </row>
-    <row r="127" spans="1:146" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:146" ht="96" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>1263</v>
       </c>
@@ -60955,7 +60955,7 @@
         <v>1576</v>
       </c>
     </row>
-    <row r="128" spans="1:146" ht="87" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:146" ht="96" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>1267</v>
       </c>
@@ -61395,7 +61395,7 @@
         <v>1577</v>
       </c>
     </row>
-    <row r="129" spans="1:146" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:146" ht="48" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>1276</v>
       </c>
@@ -61835,7 +61835,7 @@
         <v>1573</v>
       </c>
     </row>
-    <row r="130" spans="1:146" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:146" ht="112" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>1280</v>
       </c>
@@ -62275,7 +62275,7 @@
         <v>1576</v>
       </c>
     </row>
-    <row r="131" spans="1:146" ht="58" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:146" ht="48" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>1292</v>
       </c>
@@ -62715,7 +62715,7 @@
         <v>1576</v>
       </c>
     </row>
-    <row r="132" spans="1:146" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:146" ht="96" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>1300</v>
       </c>
@@ -63155,7 +63155,7 @@
         <v>1576</v>
       </c>
     </row>
-    <row r="133" spans="1:146" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:146" ht="160" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>1305</v>
       </c>
@@ -63592,7 +63592,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="134" spans="1:146" ht="58" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:146" ht="64" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>1309</v>
       </c>
@@ -64029,7 +64029,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="135" spans="1:146" ht="58" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:146" ht="64" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
         <v>1314</v>
       </c>
@@ -64469,7 +64469,7 @@
         <v>1573</v>
       </c>
     </row>
-    <row r="136" spans="1:146" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:146" ht="48" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>1317</v>
       </c>
@@ -64906,7 +64906,7 @@
         <v>1318</v>
       </c>
     </row>
-    <row r="137" spans="1:146" ht="58" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:146" ht="64" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
         <v>1319</v>
       </c>
@@ -65346,7 +65346,7 @@
         <v>1573</v>
       </c>
     </row>
-    <row r="138" spans="1:146" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:146" ht="48" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
         <v>1325</v>
       </c>
@@ -65783,7 +65783,7 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="139" spans="1:146" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:146" ht="48" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
         <v>1329</v>
       </c>
@@ -66220,7 +66220,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="140" spans="1:146" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:146" ht="128" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
         <v>1332</v>
       </c>
@@ -66657,7 +66657,7 @@
         <v>1339</v>
       </c>
     </row>
-    <row r="141" spans="1:146" ht="58" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:146" ht="64" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
         <v>1340</v>
       </c>
@@ -67094,7 +67094,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="142" spans="1:146" ht="87" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:146" ht="96" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
         <v>1343</v>
       </c>
@@ -67534,7 +67534,7 @@
         <v>1588</v>
       </c>
     </row>
-    <row r="143" spans="1:146" ht="58" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:146" ht="64" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
         <v>1348</v>
       </c>
@@ -67974,7 +67974,7 @@
         <v>1598</v>
       </c>
     </row>
-    <row r="144" spans="1:146" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:146" ht="112" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
         <v>1357</v>
       </c>
@@ -68414,7 +68414,7 @@
         <v>1583</v>
       </c>
     </row>
-    <row r="145" spans="1:146" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:146" ht="48" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
         <v>1360</v>
       </c>
@@ -68854,7 +68854,7 @@
         <v>1586</v>
       </c>
     </row>
-    <row r="146" spans="1:146" ht="116" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:146" ht="128" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
         <v>1364</v>
       </c>
@@ -69291,7 +69291,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="147" spans="1:146" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:146" ht="112" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
         <v>1373</v>
       </c>
@@ -69728,7 +69728,7 @@
         <v>1378</v>
       </c>
     </row>
-    <row r="148" spans="1:146" ht="58" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:146" ht="64" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
         <v>1379</v>
       </c>
@@ -70168,7 +70168,7 @@
         <v>1573</v>
       </c>
     </row>
-    <row r="149" spans="1:146" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:146" ht="48" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
         <v>1381</v>
       </c>
@@ -70608,7 +70608,7 @@
         <v>1576</v>
       </c>
     </row>
-    <row r="150" spans="1:146" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:146" ht="160" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
         <v>1384</v>
       </c>
@@ -71045,7 +71045,7 @@
         <v>1389</v>
       </c>
     </row>
-    <row r="151" spans="1:146" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:146" ht="48" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
         <v>1390</v>
       </c>
@@ -71482,7 +71482,7 @@
         <v>1393</v>
       </c>
     </row>
-    <row r="152" spans="1:146" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:146" ht="48" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
         <v>1394</v>
       </c>
@@ -71919,7 +71919,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="153" spans="1:146" ht="87" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:146" ht="96" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
         <v>1395</v>
       </c>
@@ -72359,7 +72359,7 @@
         <v>1580</v>
       </c>
     </row>
-    <row r="154" spans="1:146" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:146" ht="144" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
         <v>1405</v>
       </c>
@@ -72796,7 +72796,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="155" spans="1:146" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:146" ht="80" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
         <v>1417</v>
       </c>
@@ -73233,7 +73233,7 @@
         <v>1420</v>
       </c>
     </row>
-    <row r="156" spans="1:146" ht="58" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:146" ht="48" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
         <v>1421</v>
       </c>
@@ -73673,7 +73673,7 @@
         <v>1576</v>
       </c>
     </row>
-    <row r="157" spans="1:146" ht="116" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:146" ht="128" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
         <v>1422</v>
       </c>
@@ -74110,7 +74110,7 @@
         <v>1429</v>
       </c>
     </row>
-    <row r="158" spans="1:146" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:146" ht="80" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
         <v>1430</v>
       </c>
@@ -74550,7 +74550,7 @@
         <v>1592</v>
       </c>
     </row>
-    <row r="159" spans="1:146" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:146" x14ac:dyDescent="0.2">
       <c r="H159" s="1"/>
     </row>
   </sheetData>
@@ -74581,7 +74581,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId22"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:A7 B1:B2 C1:C7 D1:D7 E1:E7 F1:F3 G1:G7 I1:I7 J1:J7 K1:K2 L1:L7 M1:M2 N1:N7 O1:O3 P1:P2 Q1:Q7 R1:R2 S1:S2 T1:T7 U1:U2 V1:V7 W1:W2 X1:X2 Y1:Y2 Z1:Z2 AA1:AA2 AB1:AB2 AC1:AC2 AD1:AD2 AE1:AE2 AF1:AF2 AG1:AG7 AH1:AH2 AI1:AI2 AJ1:AJ2 AK1:AK2 AL1:AL2 AM1:AM2 AN1:AN2 AO1:AO2 AP1:AP2 AQ1:AQ2 AR1:AR7 AS1:AS2 AT1:AT2 AU1:AU2 AV1:AV2 AW1:AW2 AX1:AX2 AY1:AY2 AZ1:AZ2 BA1:BA2 BB1:BB2 BC1:BC7 BD1:BD2 BE1:BE2 BF1:BF2 BG1:BG2 BH1:BH2 BI1:BI2 BJ1:BJ2 BK1:BK2 BL1:BL2 BM1:BM2 BN1:BN7 BO1:BO2 BP1:BP2 BQ1:BQ2 BR1:BR2 BS1:BS2 BT1:BT2 BU1:BU2 BV1:BV2 BW1:BW2 BX1:BX2 BY1:BY7 BZ1:BZ2 CA1:CA2 CB1:CB2 CC1:CC2 CD1:CD2 CE1:CE2 CF1:CF2 CG1:CG2 CH1:CH2 CI1:CI2 CJ1:CJ7 CK1:CK2 CL1:CL2 CM1:CM2 CN1:CN2 CO1:CO2 CP1:CP2 CQ1:CQ2 CR1:CR2 CS1:CS2 CT1:CT2 CU1:CU7 CV1:CV2 CW1:CW2 CX1:CX2 CY1:CY2 CZ1:CZ2 DA1:DA2 DB1:DB2 DC1:DC2 DD1:DD2 DE1:DE2 DF1:DF7 DG1:DG2 DH1:DH2 DI1:DI2 DJ1:DJ2 DK1:DK2 DL1:DL2 DM1:DM2 DN1:DN2 DO1:DO2 DP1:DP2 DQ1:DQ7 DR1:DR3 DS1:DS3 DT1:DT3 DU1:DU3 DV1:DV3 DW1:DW3 DX1:DX3 DY1:DY3 DZ1:DZ3 EA1:EA3 EB1:EB7 EC1:EC2 ED1:ED2 EE1:EE2 EF1:EF2 EG1:EG2 EH1:EH2 EI1:EI2 EJ1:EJ2 EK1:EK2 EL1:EL2 EM1:EM7 EN1:EN7 EO1:EO7 EO95:EO96 EO98 EO100:EO101 EO105:EO110 EO112:EO127 EO135 EO137:EO139 EO142:EO143 EO17:EO22 EO24:EO25 EO29:EO32 EO35:EO37 EO39:EO40 EO42:EO50 EO51:EO52 EO55:EO57 EO59:EO70 EO72:EO86 A26:A32 C26:C32 D26:D32 E26:E32 F28:F32 G26:G32 I26:I32 J26:J32 L26:L28 M30:M31 N26:N32 O26 Q26:Q28 T26:T32 V26:V27 AG26:AG32 AR26:AR32 BC26:BC32 BE28 BI28 BJ28 BK28 BL28 BM28 BN26:BN32 BY26:BY32 CC30 CJ26:CJ32 CK27 CL27 CM27 CN27 CO27 CP27 CQ27 CR27 CS27 CT27 CU26:CU32 DF26:DF32 DQ26:DQ32 EB26:EB32 EM26:EM32 EN26:EN32 EO26 EO33 A33:A37 C33:C37 D33:D37 E33:E37 F37 G33:G37 I33:I37 J33:J37 L34:L36 N33:N36 O33:O37 P34:P36 Q33:Q36 R34:R37 T33:T37 V33:V37 AG33:AG37 AR33:AR37 AS37 AU37 BC33:BC37 BD35 BE35 BF35 BG35 BI35 BJ35 BK35 BL35 BN33:BN37 BY33:BY37 BZ33 CA33 CB33 CC33 CD33 CE33 CF33 CG33 CH33 CI33 CJ33:CJ37 CK34 CL34 CM34 CN34 CO34 CP34 CQ34 CR34 CS34 CT34 CU33:CU37 DF33:DF37 DQ33:DQ37 EB33:EB37 EM33:EM37 EN33:EN37 EO38 A38 C38 D38 E38 F38 G38 I38 L38 N38 O38 P38 Q38 R38 T38 V38 AG38 AR38 BC38 BN38 BY38 CJ38 CU38 DF38 DQ38 EB38 EM38 EN38 A51:A52 C51:C52 D51:D52 E51:E52 G51:G52 I51:I52 J51:J52 L51:L52 N51:N52 O51:O52 Q51:Q52 T51:T52 V51 AG51:AG52 AR51:AR52 BC51:BC52 BN51:BN52 BO52 BP52 BQ52 BR52 BS52 BT52 BU52 BV52 BW52 BX52 BY51:BY52 CJ51:CJ52 CU51:CU52 CV51 CW51 CX51 CY51 CZ51 DA51 DB51 DC51 DD51 DE51 DF51:DF52 DQ51:DQ52 EB51:EB52 EM51:EM52 EN51:EN52 EO53 A53:A86 C53:C86 D53:D86 E53:E86 F53:F58 G53:G86 I53:I86 J53:J59 L53 M55:M56 N53 O53:O59 P53 Q53:Q59 R53 T53:T86 V53:V65 AG53:AG86 AH53 AI53 AJ53 AK53 AL53 AM53 AN53 AO53 AP53 AQ53 AR53:AR86 BC53:BC86 BD54 BE54 BF54 BG54 BH54 BI54 BJ54 BK54 BL54 BM54 BN53:BN86 BY53:BY86 CJ53:CJ86 CU53:CU86 DF53:DF86 DQ53:DQ86 DR55 DS55 DT55 DV55 DW55 DX55 DZ55 EB53:EB86 EM53:EM86 EN53:EN86 EO144 A144 C144 D144 E144 G144 I144 J144 N144 O144 T144 V144 AG144 AR144 BC144 BN144 BY144 CJ144 CU144 DF144 DQ144 EB144 EM144 EN144 EO145 A145 C145 D145 E145 G145 I145 J145 L145 N145 O145 P145 Q145 R145 T145 V145 AG145 AR145 BC145 BN145 BY145 CJ145 CU145 DF145 DQ145 EB145 EM145 EN145 EO146 A146 C146 D146 E146 G146 I146 J146 N146 O146 P146 Q146 R146 T146 AG146 AR146 BC146 BN146 BY146 CJ146 CU146 DF146 DQ146 EB146 EM146 EN146 EO147 A147 C147 D147 E147 F147 G147 I147 J147 L147 N147 O147 Q147 T147 V147 AG147 AR147 BC147 BN147 BY147 CJ147 CU147 DF147 DQ147 EB147 EM147 EN147 EO148:EO149 A148:A149 C149 D148:D149 E148:E149 F149 G148:G149 I148:I149 J148:J149 L148:L149 N148:N149 O148:O149 P148:P149 Q148:Q149 R148:R149 T148:T149 V149 AG148:AG149 AR148:AR149 BC148:BC149 BN148:BN149 BY148:BY149 CJ148:CJ149 CU148:CU149 DF148:DF149 DQ148:DQ149 EB148:EB149 EM148:EM149 EN148:EN149 EO150 A150 C150 D150 E150 F150 G150 I150 J150 L150 N150 O150 Q150 T150 AG150 AR150 BC150 BN150 BY150 CJ150 CU150 DF150 DQ150 EB150 EM150 EN150 EO151:EO152 A151:A152 C151:C152 D151:D152 E151:E152 F151 G151:G152 I151:I152 J151:J152 L151:L152 N151:N152 O151:O152 Q151:Q152 R151 T151:T152 V151:V152 AG151:AG152 AR151:AR152 BC151:BC152 BN151:BN152 BY151:BY152 CJ151:CJ152 CU151:CU152 DF151:DF152 DQ151:DQ152 EB151:EB152 EM151:EM152 EN151:EN152 EO153 A153 C153 D153 E153 F153 G153 I153 J153 Q153 T153 AG153 AR153 BC153 BN153 BY153 CJ153 CU153 DF153 DQ153 EB153 EM153 EN153 EO154:EO156 A154:A156 C154:C156 D154:D156 E154:E156 F154:F155 G154:G156 I154:I156 J154:J156 L154 N154 O154:O156 P155:P156 Q154:Q156 R155:R156 T154:T156 V154:V156 AG154:AG156 AR154:AR156 BC154:BC156 BN154:BN156 BY154:BY156 CJ154:CJ156 CU154:CU156 DF154:DF156 DQ154:DQ156 EB154:EB156 EM154:EM156 EN154:EN156 EO157 A157 D157 E157 G157 I157 J157 N157 O157 P157 Q157 R157 T157 V157 AG157 AR157 BC157 BN157 BY157 CJ157 CU157 DF157 DQ157 EB157 EM157 EN157 EO158 A158 C158 D158 E158 G158 I158 J158 L158 N158 O158 Q158 T158 V158 AG158 AR158 BC158 BN158 BY158 CJ158 CU158 DF158 DQ158 EB158 EM158 EN158 EO128:EO132 A128:A143 C128:C143 D128:D143 E128:E143 F128:F132 G128:G143 I128:I143 J128:J131 L128:L141 M132 N128:N141 O128:O143 P129 Q128:Q132 R129 T128:T143 V128 AG128:AG143 AR128:AR143 BC128:BC143 BN128:BN143 BY128:BY143 CJ128:CJ143 CU128:CU143 DF128:DF143 DQ128:DQ143 EB128:EB143 EM128:EM143 EN128:EN143 A39:A50 C39:C50 D39:D50 E39:E50 F39:F41 G39:G50 I39:I45 J39:J50 L40:L44 N40:N44 O39:O50 P42:P43 Q39:Q50 T39:T50 V39:V47 AG39:AG50 AR39:AR50 AS41 AT41 AU41 AV41 AW41 AX41 AY41 AZ41 BA41 BB41 BC39:BC50 BN39:BN50 BP43 BT43 BU43 BV43 BY39:BY50 CJ39:CJ50 CU39:CU50 DF39:DF50 DQ39:DQ50 DR40 DS40 DT40 DU40 DV40 DW40 DX40 DY40 DZ40 EA40 EB39:EB50 EC39 ED39 EE39 EF39 EG39 EH39 EI39 EJ39 EK39 EL39 EM39:EM50 EN39:EN50 B115 F6:F7 F11:F12 F23:F24 F47:F50 F60 F63:F64 F69:F70 F74:F75 F79:F80 F82:F84 F87 F89 F92:F94 F96:F97 F99:F100 F102:F105 F107:F113 F115:F116 F118 F121:F123 F127 F134 F136:F140 F142 F8:F9 A8:A25 C8:C25 D8:D25 E8:E25 G8:G25 I8:I25 J8:J25 L10:L11 N9:N22 O10:O13 Q9:Q11 T8:T25 V8:V9 AG8:AG25 AR8:AR25 AY12 BB12 BC8:BC25 BN8:BN25 BP11 BR11 BS11 BT11 BU11 BV11 BW11 BY8:BY25 CJ8:CJ25 CU8:CU25 DF8:DF25 DH10 DI10 DJ10 DN10 DQ8:DQ25 DR9 DS9 DT9 DU9 DV9 DW9 DX9 DY9 DZ9 EA9 EB8:EB25 EC8 ED8 EE8 EF8 EG8 EH8 EI8 EJ8 EK8 EL8 EM8:EM25 EN8:EN25 EO8:EO15 F14:F20 M18 M60 M63:M64 M83 M91 M105 M112 M115 M136 L13 L15:L22 L24:L25 N24:N25 L31:L32 L46:L48 N46:N48 L50 N50 L55:L57 N55:N57 L59:L60 N59:N60 L62:L64 N62:N68 L66:L68 L70:L73 N70:N73 O74:O75 L76:L81 N76:N86 L83:L86 EO87:EO93 A87:A127 C87:C127 D87:D127 E87:E127 G87:G127 I87 J87:J95 Q87:Q101 R91 T87:T127 V90:V95 AG87:AG127 AR87:AR127 BC87:BC127 BN87:BN127 BY87:BY127 CJ87:CJ127 CU87:CU127 DF87:DF127 DQ87:DQ127 EB87:EB127 EM87:EM127 EN87:EN127 O87:O88 N88 L88 L90:L91 N90:N91 L93:L99 N93:N102 L104:L105 N104:N117 L107:L113 L115:L117 L121 N120:N121 J121:J123 L123:L127 N123:N127 L143 N143 L156 N156 I47:I50 I89:I127 L101 J86 J139:J143 J61:J83 J97:J101 J103:J114 J116:J118 J125:J127 J133:J137 O5:O7 O15:O25 O28:O30 O32 O61:O63 O65:O68 O70:O72 O77:O83 O85:O86 O93:O96 O98:O106 O108:O109 O111:O122 O124:O125 O127 P7 P19 P21:P22 P31 P47 P63:P64 P71:P72 P78 P83:P85 P91 P94 P98:P99 P101 P111 P124:P127 P136 P138:P139 P67 P80 P96 P114:P115 P117 P119 P104 P141 Q14:Q15 Q17:Q19 Q21:Q25 Q31:Q32 Q61:Q64 Q66:Q74 Q76:Q81 Q83:Q86 Q104:Q106 Q109 Q111:Q112 Q114:Q127 Q134:Q139 Q141:Q143 R7 R19 R42:R43 R47 R63:R64 R67 R71:R72 R78 R80:R81 R94 R96 R101 R104 R111 R124:R127 R136 R138:R139 R31 R21:R22 R83:R85 R98:R99 R113:R115 R117 R119 R141 S29 S48 S108 U72 U80 V11:V12 V15 V17 V19:V24 V29:V32 V49 V67 V70:V74 V76 V78:V83 V85:V86 V97:V100 V102 V104:V106 V109:V112 V114 V116:V118 V120:V127 V130:V131 V133:V134 V136:V143 AV4 BS6 BT6 BX6 DC5 DE5 BP6 BV6 CW5 CZ5 BO6 BQ6 DS7 DZ7 EA7 AS12 AX12 AZ12 BA12 CO13 DG10 DK10 DL10 DM10 DO10 DP10 BF14 BO11 BQ11 BX11 CS13 CV15 BH14 BI14 BM14 BX16 CG19 CQ13 DB15 DE15 BD14 BG14 BJ14 BT16 BU16 BW16 CY15 BQ16 DC15 BS16 AJ22 BF17:BF18 BG17:BG18 CD19 CH19 DB23 AK22 CC19 CF19 CI19 CZ23 AN22 AP22 AQ22 BQ21 BR21 BS21 BU21 BV21 BW21 BX21 DC23 BZ24 CW23 AL22 DE23 CI24 CV23 CX23 CY23 DA23 CA24 CC24 CD24 CE24 CG24 BF28 BG28 BH28 CE30 CF30 BZ30 CH30 CI30 CN29 CQ29 BE31 BG31 BH31 BI31 BH35 BM35 AV37 CN36 BS43 CY44 BW43 BX43 CW44 CX44 DK42 DL42 DM42 DN42 DP42 BO43 BR43 CG47 CI47 DA44 DC44 DE44 DH46 DL46 DM46 DO46 DP46 EG45 EH45 EI45 EJ45 EK45 EC45 BG48 CA47 CC47 DN46 BE48 BI48 BJ48 CB47 CE47 CH47 DC49 BH48 CV49 CW49 CX49 CZ49 DE49 CH50 DU55 EA55 AT4 CY5 DD5 BW6 CX5 DA5 DB5 BR6 DU7 DV7 AT12 AW12 BL14 CX15 DA15 BO16 BZ19 CB19 BO21 DD23 CB24 CF24 CH24 BD28 CA30 CG30 CO29 BK31 BL31 CN32 DG42 DH42 DO42 BQ43 CV44 DB44 DD44 DK46 BF48 BM48 BZ47 DI46 BK48 BL48 CD47 CF47 DB49 DD49 BD48 BZ50 CA50 CB50 CG50 CY49 DA49 CC50 CD50 AS4 DR7 DT7 DX7 DW7 CK13 CL13 CM13 CR13 CT13 BR16 AH22 AI22 AO22 BP21 AM22 CA19 CE19 CK32 CL32 CM32 CO32 CP32 CQ32 CR32 CS32 CT32 AT37 AW37 AX37 AY37 AZ37 BA37 BB37 CK36 CL36 CM36 CO36 CP36 CQ36 CR36 CS36 CT36 DI42 DJ42 ED45 DJ46 DG46 CE50 DY55 CW15 AV12 BV16 CZ15 DD15 BD31 BF31 CD30 AU12 CN13 BE14 BK14 BP16 CP13 BM17:BM18 BJ31 BM31 CB30 CZ44 EE45 EF45 EL45 CF50 CI50 AU4 AW4 AX4 AY4 AZ4 BA4 BB4 BU6 CV5 DY7 BD17:BD18 BE17:BE18 BH17:BH18 BI17:BI18 BJ17:BJ18 BK17:BK18 BL17:BL18 BT21 CK29 CL29 CM29 CP29 CR29 CS29 CT29" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:A7 B1:B2 C1:C7 D1:D7 E1:E7 F1:F3 G1:G7 I1:I7 J1:J7 K1:K2 L1:L7 M1:M2 N1:N7 O1:O3 P1 Q1:Q7 R1:R2 S1:S2 T1:T7 U1:U2 V1:V7 W1:W2 X1:X2 Y1:Y2 Z1:Z2 AA1:AA2 AB1:AB2 AC1:AC2 AD1:AD2 AE1:AE2 AF1:AF2 AG1:AG7 AH1:AH2 AI1:AI2 AJ1:AJ2 AK1:AK2 AL1:AL2 AM1:AM2 AN1:AN2 AO1:AO2 AP1:AP2 AQ1:AQ2 AR1:AR7 AS1:AS2 AT1:AT2 AU1:AU2 AV1:AV2 AW1:AW2 AX1:AX2 AY1:AY2 AZ1:AZ2 BA1:BA2 BB1:BB2 BC1:BC7 BD1:BD2 BE1:BE2 BF1:BF2 BG1:BG2 BH1:BH2 BI1:BI2 BJ1:BJ2 BK1:BK2 BL1:BL2 BM1:BM2 BN1:BN7 BO1:BO2 BP1:BP2 BQ1:BQ2 BR1:BR2 BS1:BS2 BT1:BT2 BU1:BU2 BV1:BV2 BW1:BW2 BX1:BX2 BY1:BY7 BZ1:BZ2 CA1:CA2 CB1:CB2 CC1:CC2 CD1:CD2 CE1:CE2 CF1:CF2 CG1:CG2 CH1:CH2 CI1:CI2 CJ1:CJ7 CK1:CK2 CL1:CL2 CM1:CM2 CN1:CN2 CO1:CO2 CP1:CP2 CQ1:CQ2 CR1:CR2 CS1:CS2 CT1:CT2 CU1:CU7 CV1:CV2 CW1:CW2 CX1:CX2 CY1:CY2 CZ1:CZ2 DA1:DA2 DB1:DB2 DC1:DC2 DD1:DD2 DE1:DE2 DF1:DF7 DG1:DG2 DH1:DH2 DI1:DI2 DJ1:DJ2 DK1:DK2 DL1:DL2 DM1:DM2 DN1:DN2 DO1:DO2 DP1:DP2 DQ1:DQ7 DR1:DR3 DS1:DS3 DT1:DT3 DU1:DU3 DV1:DV3 DW1:DW3 DX1:DX3 DY1:DY3 DZ1:DZ3 EA1:EA3 EB1:EB7 EC1:EC2 ED1:ED2 EE1:EE2 EF1:EF2 EG1:EG2 EH1:EH2 EI1:EI2 EJ1:EJ2 EK1:EK2 EL1:EL2 EM1:EM7 EN1:EN7 EO1:EO7 EO95:EO96 EO98 EO100:EO101 EO105:EO110 EO112:EO127 EO135 EO137:EO139 EO142:EO143 EO17:EO22 EO24:EO25 EO29:EO32 EO35:EO37 EO39:EO40 EO42:EO50 EO51:EO52 EO55:EO57 EO59:EO70 EO72:EO86 A26:A32 C26:C32 D26:D32 E26:E32 F28:F32 G26:G32 I26:I32 J26:J32 L26:L28 M30:M31 N26:N32 O26 Q26:Q28 T26:T32 V26:V27 AG26:AG32 AR26:AR32 BC26:BC32 BE28 BI28 BJ28 BK28 BL28 BM28 BN26:BN32 BY26:BY32 CC30 CJ26:CJ32 CK27 CL27 CM27 CN27 CO27 CP27 CQ27 CR27 CS27 CT27 CU26:CU32 DF26:DF32 DQ26:DQ32 EB26:EB32 EM26:EM32 EN26:EN32 EO26 EO33 A33:A37 C33:C37 D33:D37 E33:E37 F37 G33:G37 I33:I37 J33:J37 L34:L36 N33:N36 O33:O37 P34:P36 Q33:Q36 R34:R37 T33:T37 V33:V37 AG33:AG37 AR33:AR37 AS37 AU37 BC33:BC37 BD35 BE35 BF35 BG35 BI35 BJ35 BK35 BL35 BN33:BN37 BY33:BY37 BZ33 CA33 CB33 CC33 CD33 CE33 CF33 CG33 CH33 CI33 CJ33:CJ37 CK34 CL34 CM34 CN34 CO34 CP34 CQ34 CR34 CS34 CT34 CU33:CU37 DF33:DF37 DQ33:DQ37 EB33:EB37 EM33:EM37 EN33:EN37 EO38 A38 C38 D38 E38 F38 G38 I38 L38 N38 O38 P38 Q38 R38 T38 V38 AG38 AR38 BC38 BN38 BY38 CJ38 CU38 DF38 DQ38 EB38 EM38 EN38 A51:A52 C51:C52 D51:D52 E51:E52 G51:G52 I51:I52 J51:J52 L51:L52 N51:N52 O51:O52 Q51:Q52 T51:T52 V51 AG51:AG52 AR51:AR52 BC51:BC52 BN51:BN52 BO52 BP52 BQ52 BR52 BS52 BT52 BU52 BV52 BW52 BX52 BY51:BY52 CJ51:CJ52 CU51:CU52 CV51 CW51 CX51 CY51 CZ51 DA51 DB51 DC51 DD51 DE51 DF51:DF52 DQ51:DQ52 EB51:EB52 EM51:EM52 EN51:EN52 EO53 A53:A86 C53:C86 D53:D86 E53:E86 F53:F58 G53:G86 I53:I86 J53:J59 L53 M55:M56 N53 O53:O59 P53 Q53:Q59 R53 T53:T86 V53:V65 AG53:AG86 AH53 AI53 AJ53 AK53 AL53 AM53 AN53 AO53 AP53 AQ53 AR53:AR86 BC53:BC86 BD54 BE54 BF54 BG54 BH54 BI54 BJ54 BK54 BL54 BM54 BN53:BN86 BY53:BY86 CJ53:CJ86 CU53:CU86 DF53:DF86 DQ53:DQ86 DR55 DS55 DT55 DV55 DW55 DX55 DZ55 EB53:EB86 EM53:EM86 EN53:EN86 EO144 A144 C144 D144 E144 G144 I144 J144 N144 O144 T144 V144 AG144 AR144 BC144 BN144 BY144 CJ144 CU144 DF144 DQ144 EB144 EM144 EN144 EO145 A145 C145 D145 E145 G145 I145 J145 L145 N145 O145 P145 Q145 R145 T145 V145 AG145 AR145 BC145 BN145 BY145 CJ145 CU145 DF145 DQ145 EB145 EM145 EN145 EO146 A146 C146 D146 E146 G146 I146 J146 N146 O146 P146 Q146 R146 T146 AG146 AR146 BC146 BN146 BY146 CJ146 CU146 DF146 DQ146 EB146 EM146 EN146 EO147 A147 C147 D147 E147 F147 G147 I147 J147 L147 N147 O147 Q147 T147 V147 AG147 AR147 BC147 BN147 BY147 CJ147 CU147 DF147 DQ147 EB147 EM147 EN147 EO148:EO149 A148:A149 C149 D148:D149 E148:E149 F149 G148:G149 I148:I149 J148:J149 L148:L149 N148:N149 O148:O149 P148:P149 Q148:Q149 R148:R149 T148:T149 V149 AG148:AG149 AR148:AR149 BC148:BC149 BN148:BN149 BY148:BY149 CJ148:CJ149 CU148:CU149 DF148:DF149 DQ148:DQ149 EB148:EB149 EM148:EM149 EN148:EN149 EO150 A150 C150 D150 E150 F150 G150 I150 J150 L150 N150 O150 Q150 T150 AG150 AR150 BC150 BN150 BY150 CJ150 CU150 DF150 DQ150 EB150 EM150 EN150 EO151:EO152 A151:A152 C151:C152 D151:D152 E151:E152 F151 G151:G152 I151:I152 J151:J152 L151:L152 N151:N152 O151:O152 Q151:Q152 R151 T151:T152 V151:V152 AG151:AG152 AR151:AR152 BC151:BC152 BN151:BN152 BY151:BY152 CJ151:CJ152 CU151:CU152 DF151:DF152 DQ151:DQ152 EB151:EB152 EM151:EM152 EN151:EN152 EO153 A153 C153 D153 E153 F153 G153 I153 J153 Q153 T153 AG153 AR153 BC153 BN153 BY153 CJ153 CU153 DF153 DQ153 EB153 EM153 EN153 EO154:EO156 A154:A156 C154:C156 D154:D156 E154:E156 F154:F155 G154:G156 I154:I156 J154:J156 L154 N154 O154:O156 P155:P156 Q154:Q156 R155:R156 T154:T156 V154:V156 AG154:AG156 AR154:AR156 BC154:BC156 BN154:BN156 BY154:BY156 CJ154:CJ156 CU154:CU156 DF154:DF156 DQ154:DQ156 EB154:EB156 EM154:EM156 EN154:EN156 EO157 A157 D157 E157 G157 I157 J157 N157 O157 P157 Q157 R157 T157 V157 AG157 AR157 BC157 BN157 BY157 CJ157 CU157 DF157 DQ157 EB157 EM157 EN157 EO158 A158 C158 D158 E158 G158 I158 J158 L158 N158 O158 Q158 T158 V158 AG158 AR158 BC158 BN158 BY158 CJ158 CU158 DF158 DQ158 EB158 EM158 EN158 EO128:EO132 A128:A143 C128:C143 D128:D143 E128:E143 F128:F132 G128:G143 I128:I143 J128:J131 L128:L141 M132 N128:N141 O128:O143 P129 Q128:Q132 R129 T128:T143 V128 AG128:AG143 AR128:AR143 BC128:BC143 BN128:BN143 BY128:BY143 CJ128:CJ143 CU128:CU143 DF128:DF143 DQ128:DQ143 EB128:EB143 EM128:EM143 EN128:EN143 A39:A50 C39:C50 D39:D50 E39:E50 F39:F41 G39:G50 I39:I45 J39:J50 L40:L44 N40:N44 O39:O50 P42:P43 Q39:Q50 T39:T50 V39:V47 AG39:AG50 AR39:AR50 AS41 AT41 AU41 AV41 AW41 AX41 AY41 AZ41 BA41 BB41 BC39:BC50 BN39:BN50 BP43 BT43 BU43 BV43 BY39:BY50 CJ39:CJ50 CU39:CU50 DF39:DF50 DQ39:DQ50 DR40 DS40 DT40 DU40 DV40 DW40 DX40 DY40 DZ40 EA40 EB39:EB50 EC39 ED39 EE39 EF39 EG39 EH39 EI39 EJ39 EK39 EL39 EM39:EM50 EN39:EN50 B115 F6:F7 F11:F12 F23:F24 F47:F50 F60 F63:F64 F69:F70 F74:F75 F79:F80 F82:F84 F87 F89 F92:F94 F96:F97 F99:F100 F102:F105 F107:F113 F115:F116 F118 F121:F123 F127 F134 F136:F140 F142 F8:F9 A8:A25 C8:C25 D8:D25 E8:E25 G8:G25 I8:I25 J8:J25 L10:L11 N9:N22 O10:O13 Q9:Q11 T8:T25 V8:V9 AG8:AG25 AR8:AR25 AY12 BB12 BC8:BC25 BN8:BN25 BP11 BR11 BS11 BT11 BU11 BV11 BW11 BY8:BY25 CJ8:CJ25 CU8:CU25 DF8:DF25 DH10 DI10 DJ10 DN10 DQ8:DQ25 DR9 DS9 DT9 DU9 DV9 DW9 DX9 DY9 DZ9 EA9 EB8:EB25 EC8 ED8 EE8 EF8 EG8 EH8 EI8 EJ8 EK8 EL8 EM8:EM25 EN8:EN25 EO8:EO15 F14:F20 M18 M60 M63:M64 M83 M91 M105 M112 M115 M136 L13 L15:L22 L24:L25 N24:N25 L31:L32 L46:L48 N46:N48 L50 N50 L55:L57 N55:N57 L59:L60 N59:N60 L62:L64 N62:N68 L66:L68 L70:L73 N70:N73 O74:O75 L76:L81 N76:N86 L83:L86 EO87:EO93 A87:A127 C87:C127 D87:D127 E87:E127 G87:G127 I87 J87:J95 Q87:Q101 R91 T87:T127 V90:V95 AG87:AG127 AR87:AR127 BC87:BC127 BN87:BN127 BY87:BY127 CJ87:CJ127 CU87:CU127 DF87:DF127 DQ87:DQ127 EB87:EB127 EM87:EM127 EN87:EN127 O87:O88 N88 L88 L90:L91 N90:N91 L93:L99 N93:N102 L104:L105 N104:N117 L107:L113 L115:L117 L121 N120:N121 J121:J123 L123:L127 N123:N127 L143 N143 L156 N156 I47:I50 I89:I127 L101 J86 J139:J143 J61:J83 J97:J101 J103:J114 J116:J118 J125:J127 J133:J137 O5:O7 O15:O25 O28:O30 O32 O61:O63 O65:O68 O70:O72 O77:O83 O85:O86 O93:O96 O98:O106 O108:O109 O111:O122 O124:O125 O127 P7 P19 P21:P22 P31 P47 P63:P64 P71:P72 P78 P83:P85 P91 P94 P98:P99 P101 P111 P124:P127 P136 P138:P139 P67 P80 P96 P114:P115 P117 P119 P104 P141 Q14:Q15 Q17:Q19 Q21:Q25 Q31:Q32 Q61:Q64 Q66:Q74 Q76:Q81 Q83:Q86 Q104:Q106 Q109 Q111:Q112 Q114:Q127 Q134:Q139 Q141:Q143 R7 R19 R42:R43 R47 R63:R64 R67 R71:R72 R78 R80:R81 R94 R96 R101 R104 R111 R124:R127 R136 R138:R139 R31 R21:R22 R83:R85 R98:R99 R113:R115 R117 R119 R141 S29 S48 S108 U72 U80 V11:V12 V15 V17 V19:V24 V29:V32 V49 V67 V70:V74 V76 V78:V83 V85:V86 V97:V100 V102 V104:V106 V109:V112 V114 V116:V118 V120:V127 V130:V131 V133:V134 V136:V143 AV4 BS6 BT6 BX6 DC5 DE5 BP6 BV6 CW5 CZ5 BO6 BQ6 DS7 DZ7 EA7 AS12 AX12 AZ12 BA12 CO13 DG10 DK10 DL10 DM10 DO10 DP10 BF14 BO11 BQ11 BX11 CS13 CV15 BH14 BI14 BM14 BX16 CG19 CQ13 DB15 DE15 BD14 BG14 BJ14 BT16 BU16 BW16 CY15 BQ16 DC15 BS16 AJ22 BF17:BF18 BG17:BG18 CD19 CH19 DB23 AK22 CC19 CF19 CI19 CZ23 AN22 AP22 AQ22 BQ21 BR21 BS21 BU21 BV21 BW21 BX21 DC23 BZ24 CW23 AL22 DE23 CI24 CV23 CX23 CY23 DA23 CA24 CC24 CD24 CE24 CG24 BF28 BG28 BH28 CE30 CF30 BZ30 CH30 CI30 CN29 CQ29 BE31 BG31 BH31 BI31 BH35 BM35 AV37 CN36 BS43 CY44 BW43 BX43 CW44 CX44 DK42 DL42 DM42 DN42 DP42 BO43 BR43 CG47 CI47 DA44 DC44 DE44 DH46 DL46 DM46 DO46 DP46 EG45 EH45 EI45 EJ45 EK45 EC45 BG48 CA47 CC47 DN46 BE48 BI48 BJ48 CB47 CE47 CH47 DC49 BH48 CV49 CW49 CX49 CZ49 DE49 CH50 DU55 EA55 AT4 CY5 DD5 BW6 CX5 DA5 DB5 BR6 DU7 DV7 AT12 AW12 BL14 CX15 DA15 BO16 BZ19 CB19 BO21 DD23 CB24 CF24 CH24 BD28 CA30 CG30 CO29 BK31 BL31 CN32 DG42 DH42 DO42 BQ43 CV44 DB44 DD44 DK46 BF48 BM48 BZ47 DI46 BK48 BL48 CD47 CF47 DB49 DD49 BD48 BZ50 CA50 CB50 CG50 CY49 DA49 CC50 CD50 AS4 DR7 DT7 DX7 DW7 CK13 CL13 CM13 CR13 CT13 BR16 AH22 AI22 AO22 BP21 AM22 CA19 CE19 CK32 CL32 CM32 CO32 CP32 CQ32 CR32 CS32 CT32 AT37 AW37 AX37 AY37 AZ37 BA37 BB37 CK36 CL36 CM36 CO36 CP36 CQ36 CR36 CS36 CT36 DI42 DJ42 ED45 DJ46 DG46 CE50 DY55 CW15 AV12 BV16 CZ15 DD15 BD31 BF31 CD30 AU12 CN13 BE14 BK14 BP16 CP13 BM17:BM18 BJ31 BM31 CB30 CZ44 EE45 EF45 EL45 CF50 CI50 AU4 AW4 AX4 AY4 AZ4 BA4 BB4 BU6 CV5 DY7 BD17:BD18 BE17:BE18 BH17:BH18 BI17:BI18 BJ17:BJ18 BK17:BK18 BL17:BL18 BT21 CK29 CL29 CM29 CP29 CR29 CS29 CT29" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>